<commit_message>
extrema functions (gradient ascent/descent, higher-order derivatives)
extrema functions (gradient ascent/descent, higher-order derivatives)
</commit_message>
<xml_diff>
--- a/src/Mathematics/Workbooks/Working.xlsx
+++ b/src/Mathematics/Workbooks/Working.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5069C9-CB2B-48C2-842B-837723DA1889}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +71,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -207,7 +208,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -561,7 +562,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>